<commit_message>
first two submissions notes (track 1)
</commit_message>
<xml_diff>
--- a/submissions.xlsx
+++ b/submissions.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/m/IDAO2020/IDAO-2020/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4E458591-441D-4D4C-9216-CAA437608CC3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0B3E407-3B0C-5F48-959F-867B5F14977F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="920" yWindow="460" windowWidth="24600" windowHeight="15000" xr2:uid="{DCA56763-5A2D-1C42-84D7-051F35045D3D}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Track 1" sheetId="1" r:id="rId1"/>
+    <sheet name="Track 2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -24,15 +25,72 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
+  <si>
+    <t>Track 1</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Score</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>Track 2</t>
+  </si>
+  <si>
+    <t>#</t>
+  </si>
+  <si>
+    <t>26.56</t>
+  </si>
+  <si>
+    <t>mb</t>
+  </si>
+  <si>
+    <t>remove time jumps, stretch all predictors vertically and horizontally</t>
+  </si>
+  <si>
+    <t>55.24</t>
+  </si>
+  <si>
+    <t>ma</t>
+  </si>
+  <si>
+    <t>IDAO example submission</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -56,8 +114,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -372,12 +432,99 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6431C626-B4BA-7948-B7AE-A0BDF1CBF28B}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:4" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" s="2" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A5FC9C4-A205-5345-9380-09A472EB05EE}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+    </row>
+    <row r="2" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
first two submissions notes (track 1), typo fixed
</commit_message>
<xml_diff>
--- a/submissions.xlsx
+++ b/submissions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/m/IDAO2020/IDAO-2020/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0B3E407-3B0C-5F48-959F-867B5F14977F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{759236A1-BE0C-9942-BC13-A21C77C14493}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="920" yWindow="460" windowWidth="24600" windowHeight="15000" xr2:uid="{DCA56763-5A2D-1C42-84D7-051F35045D3D}"/>
   </bookViews>
@@ -55,13 +55,13 @@
     <t>remove time jumps, stretch all predictors vertically and horizontally</t>
   </si>
   <si>
-    <t>55.24</t>
-  </si>
-  <si>
     <t>ma</t>
   </si>
   <si>
     <t>IDAO example submission</t>
+  </si>
+  <si>
+    <t>66.24</t>
   </si>
 </sst>
 </file>
@@ -435,7 +435,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -478,13 +478,13 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
         <v>9</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>10</v>
-      </c>
-      <c r="D4" t="s">
-        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>